<commit_message>
Added reports and some negative scenarios for sign in and create account features
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/ContactUsTestData.xlsx
+++ b/src/test/resources/testdata/ContactUsTestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sebvettal/eclipse-workspace/AutomationPractice/src/test/resources/testdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25120686-9398-5947-8375-B5B89C844D9B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E856F968-D524-6140-BAAE-07EF655F6C68}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="36120" yWindow="-620" windowWidth="27640" windowHeight="15860" xr2:uid="{563A1532-D81B-1C4A-898C-FD7DD10D7C3A}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
   <si>
     <t>SubjectHeading</t>
   </si>
@@ -430,7 +430,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -466,9 +466,6 @@
       <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
       <c r="D2" t="s">
         <v>7</v>
       </c>

</xml_diff>